<commit_message>
[refs #296242] Aggregate customs procedure from certex data
</commit_message>
<xml_diff>
--- a/cache_registry/fixtures/multi_year_licenses/combined_nomenclature.xlsx
+++ b/cache_registry/fixtures/multi_year_licenses/combined_nomenclature.xlsx
@@ -1156,8 +1156,8 @@
   </sheetPr>
   <dimension ref="A1:JA310"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A295" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B315" activeCellId="0" sqref="B315"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C314" activeCellId="0" sqref="C314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1165,7 +1165,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="5.92"/>
   </cols>
   <sheetData>

</xml_diff>